<commit_message>
07-13-23 15:26 [Added leaderboards]
</commit_message>
<xml_diff>
--- a/GUI/final project/data.xlsx
+++ b/GUI/final project/data.xlsx
@@ -415,10 +415,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:D2"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -443,78 +443,6 @@
         <is>
           <t>question by</t>
         </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>How long does the universe exists?</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>13.4 billion years</t>
-        </is>
-      </c>
-      <c r="C2" t="b">
-        <v>0</v>
-      </c>
-      <c r="D2" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>What year was python first created?</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>1991</t>
-        </is>
-      </c>
-      <c r="C3" t="b">
-        <v>0</v>
-      </c>
-      <c r="D3" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>From what year does tkinter released?</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>1991</t>
-        </is>
-      </c>
-      <c r="C4" t="b">
-        <v>0</v>
-      </c>
-      <c r="D4" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Its location has the same number as the speed of light, what structure is this?</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Pyramid of Giza</t>
-        </is>
-      </c>
-      <c r="C5" t="b">
-        <v>1</v>
-      </c>
-      <c r="D5" t="n">
-        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -531,7 +459,7 @@
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:D2"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -569,13 +497,17 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <cols>
+    <col width="15.7109375" bestFit="1" customWidth="1" min="2" max="2"/>
+    <col width="67.42578125" bestFit="1" customWidth="1" min="3" max="3"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
@@ -593,22 +525,90 @@
           <t>password</t>
         </is>
       </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>score</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>5dg2j</t>
+          <t>vfm4w</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Mikaella Aloa</t>
+          <t>Aloa, Mikaella</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
           <t>8349c112e6b9b83a9296d60d1f7783551ebe7941c2ddab7597ccd727f338bf81</t>
         </is>
+      </c>
+      <c r="D2" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2n55d</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Kimmy, Rheign</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>8349c112e6b9b83a9296d60d1f7783551ebe7941c2ddab7597ccd727f338bf81</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>g1kwu</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Rye, Rhianne</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>8349c112e6b9b83a9296d60d1f7783551ebe7941c2ddab7597ccd727f338bf81</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>my6xx</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Sesgundo, Ruina</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>8349c112e6b9b83a9296d60d1f7783551ebe7941c2ddab7597ccd727f338bf81</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -625,7 +625,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -655,7 +655,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Sesgundo, Ryann Kim M</t>
+          <t>Malabanan, RySes</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">

</xml_diff>

<commit_message>
07-29-23 04:31 [Final Done]
</commit_message>
<xml_diff>
--- a/GUI/final project/data.xlsx
+++ b/GUI/final project/data.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="questions" sheetId="1" state="visible" r:id="rId1"/>
@@ -415,9 +415,9 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D40"/>
+  <dimension ref="A1:D41"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
       <selection activeCell="D41" sqref="A41:D41"/>
     </sheetView>
   </sheetViews>
@@ -1065,7 +1065,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Binary</t>
+          <t>binary</t>
         </is>
       </c>
       <c r="C36" t="b">
@@ -1144,6 +1144,24 @@
         <v>0</v>
       </c>
       <c r="D40" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>Who developed telescope?</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Galileo Galilei</t>
+        </is>
+      </c>
+      <c r="C41" t="b">
+        <v>1</v>
+      </c>
+      <c r="D41" t="n">
         <v>2</v>
       </c>
     </row>
@@ -1160,7 +1178,7 @@
   </sheetPr>
   <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
@@ -1199,7 +1217,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
@@ -1456,12 +1474,12 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2xch1</t>
+          <t>x1snp</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>sample</t>
+          <t>De Mesa, Camille</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -1470,18 +1488,18 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>0</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>x1snp</t>
+          <t>09dqm</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>De Mesa, Camille</t>
+          <t>Sesgundo, Ryann Kim M</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -1490,7 +1508,27 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>2.5</v>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>p0rb2</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Sesgundo, Ryann Kim</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>15e2b0d3c33891ebb0f1ef609ec419420c20e320ce94c65fbc8c3312448eb225</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
12/1/2023 4:36:28 PM [autogit]
</commit_message>
<xml_diff>
--- a/GUI/final project/data.xlsx
+++ b/GUI/final project/data.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="questions" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="archives questions" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="students" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="teachers" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="questions" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="archives questions" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="students" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="teachers" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>

</xml_diff>

<commit_message>
12/1/2023 4:37:08 PM [autogit]
</commit_message>
<xml_diff>
--- a/GUI/final project/data.xlsx
+++ b/GUI/final project/data.xlsx
@@ -1217,7 +1217,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
@@ -1529,6 +1529,26 @@
       </c>
       <c r="D15" t="n">
         <v>15</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>iepoy</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Luiz Kieth Patiag</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>ef797c8118f02dfb649607dd5d3f8c7623048c9c063d532cc95c5ed7a898a64f</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
12/1/2023 4:41:29 PM [autogit]
</commit_message>
<xml_diff>
--- a/GUI/final project/data.xlsx
+++ b/GUI/final project/data.xlsx
@@ -415,7 +415,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D41"/>
+  <dimension ref="A1:D42"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
       <selection activeCell="D41" sqref="A41:D41"/>
@@ -1163,6 +1163,21 @@
       </c>
       <c r="D41" t="n">
         <v>2</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>From what year World War II ends?</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>1945</t>
+        </is>
+      </c>
+      <c r="C42" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>